<commit_message>
Changed the status LED circuit
Changed status LEDs to a BJT driver with 5 V power supply
</commit_message>
<xml_diff>
--- a/ADF5355_VCO/BOM.xlsx
+++ b/ADF5355_VCO/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korisnik\Documents\GitHub\VCO\ADF5355_VCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E77523C-ED44-4B30-B2F0-ADC1DC254B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCDCA76-6D30-4033-B95B-C06D13948B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73344E90-B40F-4A36-8DF7-D19A4216866D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
   <si>
     <t>Component</t>
   </si>
@@ -222,6 +222,15 @@
   </si>
   <si>
     <t>81-GRM1885C2A200JA1D</t>
+  </si>
+  <si>
+    <t>863-MMBT3904LT1G</t>
+  </si>
+  <si>
+    <t>BJT transistor</t>
+  </si>
+  <si>
+    <t>General purpose BJT transistor</t>
   </si>
 </sst>
 </file>
@@ -588,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD04BF4-1589-4F96-BCC7-D8F3769943E7}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +669,7 @@
         <v>40</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F27" si="0">D3*E3</f>
+        <f t="shared" ref="F3:F29" si="0">D3*E3</f>
         <v>3.76</v>
       </c>
     </row>
@@ -885,168 +894,166 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F16" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D16" s="1"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="D17" s="1">
-        <v>0.68400000000000005</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="E17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="0"/>
-        <v>3.4200000000000004</v>
+        <f>D17*E17</f>
+        <v>0.96</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0.97199999999999998</v>
-      </c>
-      <c r="E18">
-        <v>5</v>
-      </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>4.8599999999999994</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D19" s="1">
-        <v>1.1100000000000001</v>
+        <v>0.68400000000000005</v>
       </c>
       <c r="E19">
         <v>5</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>5.5500000000000007</v>
+        <v>3.4200000000000004</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D20" s="1">
-        <v>3.12</v>
+        <v>0.97199999999999998</v>
       </c>
       <c r="E20">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
-        <v>31.200000000000003</v>
+        <v>4.8599999999999994</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.5500000000000007</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3.12</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="0"/>
+        <v>31.200000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>45</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>46</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D24" s="1">
         <v>80.069999999999993</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <v>2</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F24" s="1">
         <f t="shared" si="0"/>
         <v>160.13999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="1">
-        <v>6.27</v>
-      </c>
-      <c r="E23">
-        <v>3</v>
-      </c>
-      <c r="F23" s="1">
-        <f t="shared" si="0"/>
-        <v>18.809999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F24" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D25" s="1">
-        <v>16.2</v>
+        <v>6.27</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
-        <v>16.2</v>
+        <v>18.809999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1056,27 +1063,54 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
       <c r="F27" s="1">
         <f t="shared" si="0"/>
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E30" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="1">
-        <f>SUM(F2:F27)</f>
-        <v>295.38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E31" t="s">
+      <c r="F32" s="1">
+        <f>SUM(F2:F29)</f>
+        <v>296.33999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
         <v>40</v>
       </c>
-      <c r="F31">
-        <f>F30*7.5345</f>
-        <v>2225.54061</v>
+      <c r="F33">
+        <f>F32*7.5345</f>
+        <v>2232.7737299999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added components for LED subsystem
Added resistor values and specific resistors and LEDs to BOM for the LED subsystem

Modified .gitignore to ignore autosave file
</commit_message>
<xml_diff>
--- a/ADF5355_VCO/BOM.xlsx
+++ b/ADF5355_VCO/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korisnik\Documents\GitHub\VCO\ADF5355_VCO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Razni_projekti\VCO\VCO\ADF5355_VCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCDCA76-6D30-4033-B95B-C06D13948B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D615AAFF-C457-4727-94CB-ED2CE8B3B428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73344E90-B40F-4A36-8DF7-D19A4216866D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
   <si>
     <t>Component</t>
   </si>
@@ -231,6 +231,24 @@
   </si>
   <si>
     <t>General purpose BJT transistor</t>
+  </si>
+  <si>
+    <t>941-C4SMABGYCR34Q4S1</t>
+  </si>
+  <si>
+    <t>941-C4SMAGGYCU2W37A1</t>
+  </si>
+  <si>
+    <t>941-C4SMARGYCS4V1BB1</t>
+  </si>
+  <si>
+    <t>Blue LED</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>Red LED</t>
   </si>
 </sst>
 </file>
@@ -240,10 +258,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -279,13 +305,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -301,7 +329,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema sustava Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -597,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD04BF4-1589-4F96-BCC7-D8F3769943E7}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,7 +697,7 @@
         <v>40</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F29" si="0">D3*E3</f>
+        <f t="shared" ref="F3:F32" si="0">D3*E3</f>
         <v>3.76</v>
       </c>
     </row>
@@ -899,161 +927,176 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" t="s">
-        <v>62</v>
+        <v>68</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="D17" s="1">
-        <v>9.6000000000000002E-2</v>
+        <v>0.106</v>
       </c>
       <c r="E17">
         <v>10</v>
       </c>
       <c r="F17" s="1">
         <f>D17*E17</f>
-        <v>0.96</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
       <c r="F18" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="F18:F19" si="1">D18*E18</f>
+        <v>1.01</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0.68400000000000005</v>
+        <v>67</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.10100000000000001</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="0"/>
-        <v>3.4200000000000004</v>
+        <f t="shared" si="1"/>
+        <v>1.01</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="D20" s="1">
-        <v>0.97199999999999998</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="0"/>
-        <v>4.8599999999999994</v>
+        <f>D20*E20</f>
+        <v>0.96</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="E21">
-        <v>5</v>
-      </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>5.5500000000000007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D22" s="1">
-        <v>3.12</v>
+        <v>0.68400000000000005</v>
       </c>
       <c r="E22">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>31.200000000000003</v>
+        <v>3.4200000000000004</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.8599999999999994</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D24" s="1">
-        <v>80.069999999999993</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
-        <v>160.13999999999999</v>
+        <v>5.5500000000000007</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D25" s="1">
-        <v>6.27</v>
+        <v>3.12</v>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
-        <v>18.809999999999999</v>
+        <v>31.200000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1064,29 +1107,44 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D27" s="1">
-        <v>16.2</v>
+        <v>80.069999999999993</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="0"/>
-        <v>16.2</v>
+        <v>160.13999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="1">
+        <v>6.27</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
       <c r="F28" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18.809999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1095,25 +1153,59 @@
         <v>0</v>
       </c>
     </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="0"/>
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E32" t="s">
+      <c r="F32" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="1">
-        <f>SUM(F2:F29)</f>
-        <v>296.33999999999997</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
+      <c r="F35" s="1">
+        <f>SUM(F2:F32)</f>
+        <v>299.41999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
         <v>40</v>
       </c>
-      <c r="F33">
-        <f>F32*7.5345</f>
-        <v>2232.7737299999999</v>
+      <c r="F36">
+        <f>F35*7.5345</f>
+        <v>2255.9799899999998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added TCXO and remaining footprints
Added remaining footprints
    NX3225GD
    710X toggle switch
    SMT button

Added ClearClock AX3 TCXO symbol and footprint

Added TCXO schematic with 3 options:
    LVPECL, LVDS and HCSL
</commit_message>
<xml_diff>
--- a/ADF5355_VCO/BOM.xlsx
+++ b/ADF5355_VCO/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Razni_projekti\VCO\VCO\ADF5355_VCO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3DC0DE-DFF2-4A04-9EE3-EEAE45F5EEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9235E3F-9E7E-43BE-829D-FB52B7422651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6630" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{73344E90-B40F-4A36-8DF7-D19A4216866D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73344E90-B40F-4A36-8DF7-D19A4216866D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="105">
   <si>
     <t>Component</t>
   </si>
@@ -200,12 +200,6 @@
     <t>Crystal 8MHz</t>
   </si>
   <si>
-    <t>Crystals 8.000 MHz 12 pF</t>
-  </si>
-  <si>
-    <t>520-80-12-5PX-GM-TR</t>
-  </si>
-  <si>
     <t>Crystal 32 kHz</t>
   </si>
   <si>
@@ -291,6 +285,72 @@
   </si>
   <si>
     <t>Thin film resistor</t>
+  </si>
+  <si>
+    <t>Resistor 390R</t>
+  </si>
+  <si>
+    <t>594-MCT06030C3900FP5</t>
+  </si>
+  <si>
+    <t>344-NX3225GD8MCRA3</t>
+  </si>
+  <si>
+    <t>Crystals 8.000 MHz 8 pF</t>
+  </si>
+  <si>
+    <t>81-BLM18KG121TN1D</t>
+  </si>
+  <si>
+    <t>Ferrite bead</t>
+  </si>
+  <si>
+    <t>81-LQG15HH7N5G02D</t>
+  </si>
+  <si>
+    <t>RF inductor</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>710-434781025816</t>
+  </si>
+  <si>
+    <t>SPDT Switch</t>
+  </si>
+  <si>
+    <t>611-7101TPCBE</t>
+  </si>
+  <si>
+    <t>815-AX3PAF1-125.0000</t>
+  </si>
+  <si>
+    <t>815-AX3HAF1135.0000T</t>
+  </si>
+  <si>
+    <t>815-AX3DAF1-125.0000</t>
+  </si>
+  <si>
+    <t>Clock</t>
+  </si>
+  <si>
+    <t>603-RT0603FRE0733RL</t>
+  </si>
+  <si>
+    <t>Resistor 33R</t>
+  </si>
+  <si>
+    <t>Resistor 127R</t>
+  </si>
+  <si>
+    <t>Resistor 82R5</t>
+  </si>
+  <si>
+    <t>603-RT0603FRE07127RL</t>
+  </si>
+  <si>
+    <t>594-MCT06030C8259FP5</t>
   </si>
 </sst>
 </file>
@@ -667,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD04BF4-1589-4F96-BCC7-D8F3769943E7}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,7 +799,7 @@
         <v>40</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F38" si="0">D3*E3</f>
+        <f t="shared" ref="F3:F51" si="0">D3*E3</f>
         <v>3.76</v>
       </c>
     </row>
@@ -808,13 +868,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
         <v>59</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>61</v>
       </c>
       <c r="D7" s="1">
         <v>4.1000000000000002E-2</v>
@@ -850,10 +910,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D9" s="4">
         <v>0.104</v>
@@ -868,10 +928,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" s="1">
         <v>0.03</v>
@@ -886,10 +946,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D11" s="1">
         <v>4.3999999999999997E-2</v>
@@ -970,13 +1030,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D16" s="1">
         <v>0.04</v>
@@ -991,13 +1051,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D17" s="1">
         <v>6.3E-2</v>
@@ -1012,13 +1072,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D18" s="1">
         <v>6.3E-2</v>
@@ -1032,308 +1092,322 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="A19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="1">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E19">
+        <v>20</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" ref="F19" si="1">D19*E19</f>
+        <v>1.26</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="D20" s="1">
-        <v>0.33800000000000002</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="E20">
         <v>10</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="0"/>
-        <v>3.3800000000000003</v>
+        <f>D20*E20</f>
+        <v>0.29000000000000004</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="D21" s="1">
-        <v>1.1399999999999999</v>
+        <v>0.05</v>
       </c>
       <c r="E21">
         <v>10</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="0"/>
-        <v>11.399999999999999</v>
+        <f t="shared" ref="F21:F23" si="2">D21*E21</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="A22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.115</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="2"/>
+        <v>1.1500000000000001</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0.106</v>
-      </c>
-      <c r="E23">
-        <v>10</v>
-      </c>
+      <c r="D23" s="1"/>
       <c r="F23" s="1">
-        <f>D23*E23</f>
-        <v>1.06</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="E24">
-        <v>10</v>
-      </c>
-      <c r="F24" s="1">
-        <f t="shared" ref="F24:F25" si="1">D24*E24</f>
-        <v>1.01</v>
-      </c>
+      <c r="D24" s="1"/>
+      <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="4">
-        <v>0.10100000000000001</v>
+        <v>89</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.184</v>
       </c>
       <c r="E25">
         <v>10</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="1"/>
-        <v>1.01</v>
+        <f>D25*E25</f>
+        <v>1.8399999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="D26" s="1">
-        <v>9.6000000000000002E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="E26">
         <v>10</v>
       </c>
       <c r="F26" s="1">
         <f>D26*E26</f>
-        <v>0.96</v>
+        <v>0.57000000000000006</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F27" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D27" s="1"/>
+      <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="D28" s="1">
-        <v>0.68400000000000005</v>
+        <v>0.64500000000000002</v>
       </c>
       <c r="E28">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="0"/>
-        <v>3.4200000000000004</v>
+        <v>6.45</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="D29" s="1">
-        <v>0.97199999999999998</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="0"/>
-        <v>4.8599999999999994</v>
+        <v>11.399999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="D30" s="1">
-        <v>1.1100000000000001</v>
+        <v>5.14</v>
       </c>
       <c r="E30">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="0"/>
-        <v>5.5500000000000007</v>
+        <v>5.14</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="D31" s="1">
-        <v>3.12</v>
+        <v>4.6100000000000003</v>
       </c>
       <c r="E31">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="0"/>
-        <v>31.200000000000003</v>
+        <v>4.6100000000000003</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="1">
+        <v>5.42</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
       <c r="F32" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.42</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="1">
-        <v>80.069999999999993</v>
-      </c>
-      <c r="E33">
-        <v>2</v>
-      </c>
-      <c r="F33" s="1">
-        <f t="shared" si="0"/>
-        <v>160.13999999999999</v>
-      </c>
+      <c r="D33" s="1"/>
+      <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" t="s">
-        <v>47</v>
+        <v>66</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="D34" s="1">
-        <v>6.27</v>
+        <v>0.106</v>
       </c>
       <c r="E34">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="0"/>
-        <v>18.809999999999999</v>
+        <f>D34*E34</f>
+        <v>1.06</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="E35">
+        <v>10</v>
+      </c>
       <c r="F35" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="F35:F36" si="3">D35*E35</f>
+        <v>1.01</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" s="1">
-        <v>16.2</v>
+        <v>65</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0.10100000000000001</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" si="0"/>
-        <v>16.2</v>
+        <f t="shared" si="3"/>
+        <v>1.01</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="1">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="E37">
+        <v>10</v>
+      </c>
       <c r="F37" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D37*E37</f>
+        <v>0.96</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1342,22 +1416,229 @@
         <v>0</v>
       </c>
     </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="F39" s="1">
+        <f>D39*E39</f>
+        <v>3.24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="1">
+        <v>15.35</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1">
+        <f>D40*E40</f>
+        <v>15.35</v>
+      </c>
+    </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E41" t="s">
+      <c r="A41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="0"/>
+        <v>3.4200000000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="0"/>
+        <v>4.8599999999999994</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="0"/>
+        <v>5.5500000000000007</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" s="1">
+        <v>3.12</v>
+      </c>
+      <c r="E44">
+        <v>10</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="0"/>
+        <v>31.200000000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" s="1">
+        <v>80.069999999999993</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="0"/>
+        <v>160.13999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="1">
+        <v>6.27</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="0"/>
+        <v>18.809999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="0"/>
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
         <v>39</v>
       </c>
-      <c r="F41" s="1">
-        <f>SUM(F2:F38)</f>
-        <v>305.26</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E42" t="s">
+      <c r="F54" s="1">
+        <f>SUM(F2:F51)</f>
+        <v>347.69999999999993</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
         <v>40</v>
       </c>
-      <c r="F42">
-        <f>F41*7.5345</f>
-        <v>2299.9814700000002</v>
+      <c r="F55">
+        <f>F54*7.5345</f>
+        <v>2619.7456499999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>